<commit_message>
with dart code of tree
</commit_message>
<xml_diff>
--- a/plant_health/plant_health_train.xlsx
+++ b/plant_health/plant_health_train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Python\Decission_Tree\plant_health\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7599579E-708C-45AE-804E-6837BAF0062F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C377AE5-B96E-43DF-8E3B-CDCF34050045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19500" yWindow="510" windowWidth="18620" windowHeight="20080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,7 +461,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>